<commit_message>
Minor updates to the importer
</commit_message>
<xml_diff>
--- a/xls-import-sample.xlsx
+++ b/xls-import-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t xml:space="preserve">№ п/п</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Объект пригоден к эксплуатации, но требует ремонта система отопления.</t>
   </si>
   <si>
-    <t xml:space="preserve">ФИО , телефон</t>
+    <t xml:space="preserve">Иванов Иван Иванович</t>
   </si>
   <si>
     <t xml:space="preserve">изображение объекта</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Объект пригоден к эксплуатации.</t>
   </si>
   <si>
-    <t xml:space="preserve">ГБУСО «Мустаевскийпсихо-неврологический интернат»</t>
+    <t xml:space="preserve">ГБУСО «Мустаевский психоневрологический интернат»</t>
   </si>
   <si>
     <t xml:space="preserve">Здание, назначение: нежилое (коровник)</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Илекский район, с. Заживное, ул. Степная, 1А</t>
   </si>
   <si>
-    <t xml:space="preserve">ГБУСО «Сакмарскийпсихоневрологичес-кий интернат»</t>
+    <t xml:space="preserve">ГБУСО «Сакмарский психоневрологический интернат»</t>
   </si>
   <si>
     <t xml:space="preserve">Здание зерносклада</t>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t xml:space="preserve">56-56-28/005/2006-030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ГБУСО «Сакмарский психо-неврологический интернат»</t>
   </si>
   <si>
     <t xml:space="preserve">Здание конюшни </t>
@@ -178,6 +181,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -198,6 +202,7 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -339,20 +344,20 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -429,7 +434,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>1</v>
       </c>
@@ -489,7 +494,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
         <v>3</v>
       </c>
@@ -519,7 +524,7 @@
       </c>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="n">
         <v>4</v>
       </c>
@@ -549,7 +554,7 @@
       </c>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
         <v>5</v>
       </c>
@@ -579,7 +584,7 @@
       </c>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="n">
         <v>6</v>
       </c>
@@ -609,7 +614,7 @@
       </c>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
         <v>7</v>
       </c>
@@ -639,7 +644,7 @@
       </c>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
         <v>8</v>
       </c>
@@ -669,15 +674,15 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>36</v>
@@ -686,7 +691,7 @@
         <v>21.8</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>38</v>
@@ -699,7 +704,7 @@
       </c>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="n">
         <v>10</v>
       </c>
@@ -707,10 +712,10 @@
         <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>515.1</v>
@@ -729,7 +734,7 @@
       </c>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="n">
         <v>11</v>
       </c>
@@ -737,16 +742,16 @@
         <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>230.7</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>38</v>

</xml_diff>